<commit_message>
reorganised repo and added new readme
</commit_message>
<xml_diff>
--- a/Notes/CAN Bus Messages.xlsx
+++ b/Notes/CAN Bus Messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigel\Documents\GitHub\evam_canbus\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panziyue/Developer/Hardware/EVAM/evam-1-canbus/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0DF584-C148-4E78-970F-FBB49A1B453E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D44259F-CAF9-0349-AFD2-5D2E92E3BBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="874" yWindow="-103" windowWidth="26657" windowHeight="15634" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="500" windowWidth="29400" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="211">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -720,6 +720,9 @@
   </si>
   <si>
     <t>5V voltage(V) = B1/36 UNCALIBRATED</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -922,19 +925,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1239,27 +1242,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="P46" sqref="P46"/>
+      <selection pane="bottomLeft" activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="30" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.84375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.3046875" customWidth="1"/>
-    <col min="14" max="14" width="13.69140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="1.53515625" style="11" customWidth="1"/>
-    <col min="16" max="16" width="22.69140625" customWidth="1"/>
-    <col min="17" max="23" width="20.53515625" customWidth="1"/>
-    <col min="28" max="28" width="100.15234375" style="5" customWidth="1"/>
-    <col min="29" max="29" width="2.53515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="12.83203125" customWidth="1"/>
+    <col min="14" max="14" width="36.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.5" style="11" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" customWidth="1"/>
+    <col min="17" max="23" width="20.5" customWidth="1"/>
+    <col min="28" max="28" width="100.1640625" style="5" customWidth="1"/>
+    <col min="29" max="29" width="2.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,17 +1277,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
       <c r="N1" s="9" t="s">
         <v>52</v>
       </c>
@@ -1319,7 +1327,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1333,7 +1341,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1344,7 +1352,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>3</v>
       </c>
@@ -1360,7 +1368,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:30" ht="32" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>4</v>
       </c>
@@ -1384,7 +1392,7 @@
       </c>
       <c r="AB6" s="6"/>
     </row>
-    <row r="7" spans="1:30" s="18" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:30" s="18" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="18">
         <v>5</v>
       </c>
@@ -1410,12 +1418,12 @@
       <c r="AB7" s="23"/>
       <c r="AC7" s="22"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>7</v>
       </c>
@@ -1435,7 +1443,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="18">
         <v>8</v>
       </c>
@@ -1461,7 +1469,7 @@
       <c r="AB10" s="21"/>
       <c r="AC10" s="22"/>
     </row>
-    <row r="11" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="18">
         <v>9</v>
       </c>
@@ -1487,7 +1495,7 @@
       <c r="AB11" s="23"/>
       <c r="AC11" s="22"/>
     </row>
-    <row r="12" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18">
         <v>10</v>
       </c>
@@ -1513,7 +1521,7 @@
       <c r="AB12" s="23"/>
       <c r="AC12" s="22"/>
     </row>
-    <row r="13" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="18">
         <v>11</v>
       </c>
@@ -1536,14 +1544,14 @@
       <c r="P13" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="Q13" s="30" t="s">
+      <c r="Q13" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="R13" s="30"/>
+      <c r="R13" s="29"/>
       <c r="AB13" s="23"/>
       <c r="AC13" s="22"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>12</v>
       </c>
@@ -1567,7 +1575,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>13</v>
       </c>
@@ -1590,12 +1598,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>15</v>
       </c>
@@ -1615,7 +1623,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>16</v>
       </c>
@@ -1635,7 +1643,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>17</v>
       </c>
@@ -1652,7 +1660,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>18</v>
       </c>
@@ -1669,7 +1677,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>19</v>
       </c>
@@ -1686,62 +1694,62 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>31</v>
       </c>
@@ -1749,7 +1757,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:30" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1791,7 +1799,7 @@
       </c>
       <c r="AB34" s="6"/>
     </row>
-    <row r="35" spans="1:30" s="12" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:30" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B35" s="12">
         <v>33</v>
       </c>
@@ -1828,7 +1836,7 @@
       </c>
       <c r="AC35" s="16"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>34</v>
       </c>
@@ -1863,12 +1871,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>36</v>
       </c>
@@ -1907,7 +1915,7 @@
       </c>
       <c r="AB38" s="6"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>37</v>
       </c>
@@ -1937,38 +1945,38 @@
       </c>
       <c r="AB39" s="6"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>38</v>
       </c>
       <c r="AB40" s="6"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:30" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>44</v>
       </c>
@@ -1990,31 +1998,31 @@
       <c r="P46" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="Q46" s="29" t="s">
+      <c r="Q46" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="R46" s="29"/>
+      <c r="R46" s="27"/>
       <c r="S46" t="s">
         <v>208</v>
       </c>
       <c r="AB46" s="6"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:29" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:29" ht="32" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>48</v>
       </c>
@@ -2061,7 +2069,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="12">
         <v>49</v>
       </c>
@@ -2082,7 +2090,7 @@
       <c r="AB51" s="17"/>
       <c r="AC51" s="16"/>
     </row>
-    <row r="52" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="12">
         <v>50</v>
       </c>
@@ -2103,7 +2111,7 @@
       <c r="AB52" s="17"/>
       <c r="AC52" s="16"/>
     </row>
-    <row r="53" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="12">
         <v>51</v>
       </c>
@@ -2124,7 +2132,7 @@
       <c r="AB53" s="17"/>
       <c r="AC53" s="16"/>
     </row>
-    <row r="54" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>52</v>
       </c>
@@ -2151,7 +2159,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="55" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>53</v>
       </c>
@@ -2172,7 +2180,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>54</v>
       </c>
@@ -2193,7 +2201,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>55</v>
       </c>
@@ -2214,7 +2222,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>56</v>
       </c>
@@ -2238,22 +2246,22 @@
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B61">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:29" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:29" ht="80" x14ac:dyDescent="0.2">
       <c r="B62">
         <v>60</v>
       </c>
@@ -2279,7 +2287,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="63" spans="2:29" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:29" ht="96" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>61</v>
       </c>
@@ -2305,17 +2313,17 @@
         <v>202</v>
       </c>
     </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B64">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B65">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:29" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>76</v>
       </c>
@@ -2355,7 +2363,7 @@
       </c>
       <c r="AC66" s="16"/>
     </row>
-    <row r="67" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="12">
         <v>65</v>
       </c>
@@ -2367,24 +2375,24 @@
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="31" t="s">
+      <c r="P67" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="Q67" s="31"/>
-      <c r="R67" s="31" t="s">
+      <c r="Q67" s="30"/>
+      <c r="R67" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="S67" s="31"/>
-      <c r="T67" s="31" t="s">
+      <c r="S67" s="30"/>
+      <c r="T67" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="U67" s="31"/>
+      <c r="U67" s="30"/>
       <c r="AB67" s="17" t="s">
         <v>118</v>
       </c>
       <c r="AC67" s="16"/>
     </row>
-    <row r="68" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="12">
         <v>66</v>
       </c>
@@ -2396,22 +2404,22 @@
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="31" t="s">
+      <c r="P68" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="Q68" s="31"/>
-      <c r="R68" s="31" t="s">
+      <c r="Q68" s="30"/>
+      <c r="R68" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="S68" s="31"/>
-      <c r="T68" s="31" t="s">
+      <c r="S68" s="30"/>
+      <c r="T68" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="U68" s="31"/>
+      <c r="U68" s="30"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
-    <row r="69" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="12">
         <v>67</v>
       </c>
@@ -2423,42 +2431,42 @@
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="31" t="s">
+      <c r="P69" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="Q69" s="31"/>
-      <c r="R69" s="31" t="s">
+      <c r="Q69" s="30"/>
+      <c r="R69" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="S69" s="31"/>
-      <c r="T69" s="31" t="s">
+      <c r="S69" s="30"/>
+      <c r="T69" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="U69" s="31"/>
+      <c r="U69" s="30"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B70">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="12">
         <v>72</v>
       </c>
@@ -2481,7 +2489,7 @@
       <c r="AB74" s="6"/>
       <c r="AC74" s="16"/>
     </row>
-    <row r="75" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="12">
         <v>73</v>
       </c>
@@ -2498,7 +2506,7 @@
       <c r="AB75" s="17"/>
       <c r="AC75" s="16"/>
     </row>
-    <row r="76" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="12">
         <v>74</v>
       </c>
@@ -2515,7 +2523,7 @@
       <c r="AB76" s="17"/>
       <c r="AC76" s="16"/>
     </row>
-    <row r="77" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="12">
         <v>75</v>
       </c>
@@ -2532,27 +2540,27 @@
       <c r="AB77" s="17"/>
       <c r="AC77" s="16"/>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B80">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B81">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:19" ht="102" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:19" ht="112" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>80</v>
       </c>
@@ -2577,12 +2585,12 @@
       <c r="Q82" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="R82" s="29" t="s">
+      <c r="R82" s="27" t="s">
         <v>174</v>
       </c>
       <c r="S82" s="28"/>
     </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>81</v>
       </c>
@@ -2593,72 +2601,72 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="84" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B84">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="85" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B85">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B86">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B87">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="88" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B88">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="90" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B90">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B91">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="92" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B92">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="93" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B93">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="94" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="95" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B96">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B97">
         <v>95</v>
       </c>
@@ -2667,7 +2675,7 @@
       </c>
       <c r="AB97" s="6"/>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>56</v>
       </c>
@@ -2702,7 +2710,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B99">
         <v>97</v>
       </c>
@@ -2734,13 +2742,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B100">
         <v>98</v>
       </c>
       <c r="S100" s="18"/>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B101">
         <v>99</v>
       </c>
@@ -2769,68 +2777,68 @@
         <v>156</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B102">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B103">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B104">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B105">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B106">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B107">
         <v>105</v>
       </c>
       <c r="AB107" s="6"/>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B108">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B109">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B110">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B111">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B112">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B113">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>188</v>
       </c>
@@ -2847,417 +2855,417 @@
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B115">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B116">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B117">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B118">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B119">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B120">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B121">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B122">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B123">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B124">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B125">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B126">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B127">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B128">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144">
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160">
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167">
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173">
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174">
         <v>172</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175">
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176">
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177">
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178">
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179">
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180">
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181">
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183">
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184">
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185">
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186">
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188">
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189">
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190">
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191">
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192">
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B193">
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B194">
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B195">
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B196">
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>57</v>
       </c>
@@ -3265,528 +3273,534 @@
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B198">
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B199">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B200">
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B201">
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B202">
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B203">
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B204">
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B205">
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B206">
         <v>204</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B207">
         <v>205</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B208">
         <v>206</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209">
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210">
         <v>208</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211">
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212">
         <v>210</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213">
         <v>211</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214">
         <v>212</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215">
         <v>213</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216">
         <v>214</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217">
         <v>215</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218">
         <v>216</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219">
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220">
         <v>218</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221">
         <v>219</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222">
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223">
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224">
         <v>222</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225">
         <v>223</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226">
         <v>224</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227">
         <v>225</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228">
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229">
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230">
         <v>228</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231">
         <v>229</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232">
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233">
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234">
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235">
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236">
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237">
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238">
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239">
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240">
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241">
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242">
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243">
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245">
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246">
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247">
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248">
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B249">
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B250">
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B251">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B252">
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253">
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B254">
         <v>252</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255">
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256">
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B257">
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258">
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B259">
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B260">
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B261">
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262">
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263">
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B264">
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B265">
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B266">
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B267">
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B268">
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B269">
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B270">
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B271">
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B272">
         <v>270</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B273">
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B274">
         <v>272</v>
       </c>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B275">
         <v>273</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B276">
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B277">
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B278">
         <v>276</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B279">
         <v>277</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B280">
         <v>278</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B281">
         <v>279</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B282">
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B283">
         <v>281</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B284">
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B285">
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B286">
         <v>284</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B287">
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B288">
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B289">
         <v>287</v>
       </c>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B290">
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B291">
         <v>289</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B292">
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B293">
         <v>291</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B294">
         <v>292</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B295">
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B296">
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B297">
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B298">
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B299">
         <v>297</v>
       </c>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B300">
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B301">
         <v>299</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="Q46:R46"/>
     <mergeCell ref="R82:S82"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="R67:S67"/>
@@ -3802,12 +3816,6 @@
     <mergeCell ref="P58:Q58"/>
     <mergeCell ref="P68:Q68"/>
     <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="Q46:R46"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
@@ -3828,18 +3836,18 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.84375" customWidth="1"/>
-    <col min="3" max="3" width="51.3828125" customWidth="1"/>
-    <col min="4" max="4" width="48.69140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>25</v>
       </c>
@@ -3850,7 +3858,7 @@
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3864,7 +3872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="102.45" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="81" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3878,7 +3886,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -3892,7 +3900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3906,7 +3914,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3920,7 +3928,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3934,7 +3942,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -3948,7 +3956,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3956,7 +3964,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3964,7 +3972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3975,7 +3983,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -3986,7 +3994,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -4000,7 +4008,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>

</xml_diff>